<commit_message>
added Danish border fence
</commit_message>
<xml_diff>
--- a/data/EU-Walls.xlsx
+++ b/data/EU-Walls.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="86">
   <si>
     <t>state1</t>
   </si>
@@ -256,6 +256,27 @@
   </si>
   <si>
     <t>https://www.reuters.com/article/us-bulgaria-swineflu/bulgaria-to-build-wild-boar-fence-on-romanian-border-idUSKBN1KE1J4</t>
+  </si>
+  <si>
+    <t>DNK</t>
+  </si>
+  <si>
+    <t>DEU</t>
+  </si>
+  <si>
+    <t>fencing</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>NYT (2018); DW (2018)</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2018/10/24/world/europe/pig-disease-denmark-swine-fever.html</t>
+  </si>
+  <si>
+    <t>https://www.dw.com/en/denmark-to-build-controversial-german-border-fence/a-45078064</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,42 +1303,48 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C7">
-        <v>1995</v>
+        <v>2019</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1">
-        <v>20</v>
+        <v>75</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>84</v>
+      </c>
+      <c r="K7" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C8">
-        <v>2015</v>
+        <v>1995</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -1326,65 +1353,59 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="G8" s="1">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C9">
-        <v>2016</v>
-      </c>
-      <c r="D9">
-        <v>2016</v>
+        <v>2015</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C10">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="D10">
-        <v>2012</v>
+        <v>2016</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -1393,33 +1414,33 @@
         <v>14</v>
       </c>
       <c r="G10" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
       </c>
       <c r="I10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C11">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="D11">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -1428,19 +1449,19 @@
         <v>14</v>
       </c>
       <c r="G11" s="1">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
       </c>
       <c r="I11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1448,7 +1469,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C12">
         <v>2015</v>
@@ -1463,59 +1484,68 @@
         <v>14</v>
       </c>
       <c r="G12" s="1">
-        <v>329</v>
+        <v>175</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
       </c>
       <c r="I12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C13">
-        <v>2017</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
+        <v>2015</v>
+      </c>
+      <c r="D13">
+        <v>2015</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>14</v>
+      </c>
+      <c r="G13" s="1">
+        <v>329</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
       </c>
       <c r="I13" t="s">
-        <v>72</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
+      </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>35</v>
       </c>
       <c r="C14">
-        <v>2015</v>
-      </c>
-      <c r="D14">
-        <v>-2019</v>
+        <v>2017</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -1523,60 +1553,54 @@
       <c r="F14" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="1">
-        <v>23</v>
-      </c>
-      <c r="H14" t="s">
-        <v>15</v>
-      </c>
       <c r="I14" t="s">
-        <v>57</v>
-      </c>
-      <c r="J14" t="s">
-        <v>58</v>
+        <v>72</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>2015</v>
       </c>
       <c r="D15">
-        <v>2016</v>
+        <v>-2019</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G15" s="1">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
       </c>
       <c r="I15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C16">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D16">
         <v>2016</v>
@@ -1587,25 +1611,25 @@
       <c r="F16" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>68</v>
+      <c r="G16" s="1">
+        <v>30</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="J16" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C17">
         <v>2016</v>
@@ -1620,20 +1644,53 @@
         <v>14</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18">
+        <v>2016</v>
+      </c>
+      <c r="D18">
+        <v>2016</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I18" t="s">
         <v>62</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J18" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J13" r:id="rId1" display="https://www.theguardian.com/world/2017/aug/24/russia-lithuania-border-fence-kaliningrad-estonia-eston-kohver; "/>
+    <hyperlink ref="J14" r:id="rId1" display="https://www.theguardian.com/world/2017/aug/24/russia-lithuania-border-fence-kaliningrad-estonia-eston-kohver; "/>
+    <hyperlink ref="J9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>